<commit_message>
Commit the modified js and jsp file.
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>用户管理</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -88,6 +88,26 @@
   </si>
   <si>
     <t>2015.11.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色对应权限列表里的移除权限的方法没有提供。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.11.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在给的需求文档里没有关于权限管理的修改的接口方法，请提供。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -573,21 +593,41 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>

</xml_diff>

<commit_message>
Question List by 孙俊杰
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -1,134 +1,135 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowWidth="13395" windowHeight="4935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
+  <si>
+    <t>编号</t>
+  </si>
+  <si>
+    <t>功能模块</t>
+  </si>
+  <si>
+    <t>问题描述</t>
+  </si>
+  <si>
+    <t>提问者</t>
+  </si>
+  <si>
+    <t>提问时间</t>
+  </si>
+  <si>
+    <t>回答者</t>
+  </si>
+  <si>
+    <t>回答时间</t>
+  </si>
   <si>
     <t>用户管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理的更新后台貌似有错，后台像是实现的和insert的操作是一样的，无论怎么操作返回的信息都是用户名已经存在。</t>
+  </si>
+  <si>
+    <t>耿晓红</t>
+  </si>
+  <si>
+    <t>2015.11.11</t>
+  </si>
+  <si>
+    <t>添加用户的时候，编号不能为空，如果为空，返回的content是序列号已经存在，这个逻辑应该是在后台实现的。</t>
   </si>
   <si>
     <t>部门管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>部门管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户管理的更新后台貌似有错，后台像是实现的和insert的操作是一样的，无论怎么操作返回的信息都是用户名已经存在。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>添加用户的时候，编号不能为空，如果为空，返回的content是序列号已经存在，这个逻辑应该是在后台实现的。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>部门更新的模块，使用put报错
  HttpResponseProxy{HTTP/1.0 405 METHOD NOT ALLOWED [Date: Wed, 11 Nov 2015 12:59:28 GMT, Server: WSGIServer/0.1 Python/2.7.6, X-Frame-Options: SAMEORIGIN, Content-Type: text/html; charset=utf-8, Allow: GET, HEAD, OPTIONS] ResponseEntityProxy{[Content-Type: text/html; charset=utf-8,Chunked: false]}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>部门删除的模块也存在和3一样的问题。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>耿晓红</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>耿晓红</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>功能模块</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>问题描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提问者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回答者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回答时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提问时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2015.11.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>角色管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>角色对应权限列表里的移除权限的方法没有提供。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2015.11.12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>权限管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>在给的需求文档里没有关于权限管理的修改的接口方法，请提供。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资讯管理,站内信管理</t>
+  </si>
+  <si>
+    <t>是否添加批量删除功能,如果没有批量删除,是否去除行号及复选框</t>
+  </si>
+  <si>
+    <t>孙俊杰</t>
+  </si>
+  <si>
+    <t>2015.11.13</t>
+  </si>
+  <si>
+    <t>评论管理</t>
+  </si>
+  <si>
+    <t>按”是否屏蔽”过滤时,返回数据不正确(即按”是否屏蔽”单条件查询结果一直返回的是所有数据”)</t>
+  </si>
+  <si>
+    <t>标签管理</t>
+  </si>
+  <si>
+    <t>是否去除分页功能</t>
+  </si>
+  <si>
+    <t>笔记管理</t>
+  </si>
+  <si>
+    <t>按”是否公开”条件查询结果不正确</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="宋体"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,31 +164,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="百分比" xfId="4" builtinId="5"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -237,71 +253,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -434,8 +450,8 @@
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
+                <a:satMod val="350000"/>
                 <a:shade val="99000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
@@ -471,203 +487,279 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="_h" fmla="val 21600"/>
+            <a:gd name="_w" fmla="val 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:pathLst>
+            <a:path w="21600" h="21600"/>
+          </a:pathLst>
+        </a:custGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:srgbClr val="9CBEE0"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="739CC3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="200000"/>
+        </a:ln>
+      </a:spPr>
+      <a:bodyPr/>
+      <a:lstStyle/>
+    </a:spDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="9" style="3"/>
-    <col min="2" max="2" width="27.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="28.875" style="3" customWidth="1"/>
-    <col min="4" max="5" width="22.25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="24.875" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="27.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="22.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="54" x14ac:dyDescent="0.15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" ht="54" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="54" x14ac:dyDescent="0.15">
+    <row r="3" ht="54" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="189" x14ac:dyDescent="0.15">
+    <row r="4" ht="189" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="5" ht="27" spans="1:7">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="6" ht="27" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+    <row r="7" ht="27" spans="1:7">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+    <row r="8" ht="27" spans="1:7">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" ht="54" spans="1:7">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" ht="27" spans="1:7">
       <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -676,7 +768,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -685,7 +777,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -694,7 +786,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -703,7 +795,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -712,7 +804,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -721,7 +813,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -730,7 +822,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -740,34 +832,40 @@
       <c r="G19" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the question to question list.
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>编号</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>2015.11.14</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源日志的接口没有提供，相关的参数也没有文档。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.11.15</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -543,7 +555,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:E12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -780,12 +792,20 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>

</xml_diff>

<commit_message>
add question to question list
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>编号</t>
   </si>
@@ -135,6 +135,26 @@
   <si>
     <t>2015.11.15</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>应用管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有找到任何有关应用管理接口的文档。请提供</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>耿晓红</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.11.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应用管理的菜单在页面上只有专题管理和精品课程管理，我们只需要这两个吗？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -555,7 +575,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D15" sqref="D15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -809,21 +829,37 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>

</xml_diff>

<commit_message>
Change the user manager page and add question to question list.
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>编号</t>
   </si>
@@ -138,6 +138,22 @@
   </si>
   <si>
     <t>应该管理的页面下只有专题管理和精品课程管理，我们是只需要这两个功能吗？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理的搜索条件中有一个教工号，这个教工号是哪个字段？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>耿晓红</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.11.16</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:E15"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -840,12 +856,20 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>

</xml_diff>

<commit_message>
commit the question list with answer
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20370" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="问题" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <extLst/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>编号</t>
   </si>
@@ -32,9 +31,6 @@
   </si>
   <si>
     <t>提问时间</t>
-  </si>
-  <si>
-    <t>回答者</t>
   </si>
   <si>
     <t>回答时间</t>
@@ -144,19 +140,139 @@
   </si>
   <si>
     <t>按编码查询，结果集中编码项有重复</t>
+  </si>
+  <si>
+    <t>该流程目前在ui端是正常的，您说的方法指什么？删除权限的接口是有的。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限接口不设修改接口，需要修改权限需要用户先删除当前权限再重新创建。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要添加批量删除功能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口问题，马上提交进行调整</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>分页功能保留</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口问题，马上提交进行调整</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>应用管理目前只有专题的接口，先做专题</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>同上</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>没看到状况，新建的正常，是否为历史数据问题。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>确认后回复</t>
+  </si>
+  <si>
+    <t>确认后回复</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>015.11.16</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>015.11.16</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>015.11.16</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新是去掉username可以更新</t>
+  </si>
+  <si>
+    <t>编号不能为空，添加用户时需要填写</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试未发现问题</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试未发现问题</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>回答</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理的搜索条件中有一个教工号，这个教工号是哪个字段？</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>耿晓红</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.11.16</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -171,8 +287,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -208,27 +331,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -243,20 +351,171 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2049" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="666750" y="352425"/>
+          <a:ext cx="9734550" cy="4695825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2050" name="图片 2" descr="rId2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="695325" y="5105400"/>
+          <a:ext cx="9858375" cy="5048250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -554,6 +813,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -586,25 +846,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
     <col min="2" max="2" width="27.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.875" style="2" customWidth="1"/>
     <col min="4" max="5" width="22.25" style="2" customWidth="1"/>
     <col min="6" max="6" width="24.875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="2"/>
+    <col min="7" max="7" width="11.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -621,309 +881,377 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" ht="54" spans="1:7">
+    </row>
+    <row r="2" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" ht="54" spans="1:7">
+      <c r="F2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" ht="189" spans="1:7">
+      <c r="F3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="189" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" ht="27" spans="1:7">
+      <c r="F4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" ht="27" spans="1:7">
+      <c r="F5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" ht="27" spans="1:7">
+      <c r="F6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="6">
+        <v>42324</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" ht="27" spans="1:7">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="6">
+        <v>42324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" ht="54" spans="1:7">
+      <c r="F8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="6">
+        <v>42324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="6">
+        <v>42324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" ht="27" spans="1:7">
+      <c r="F10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="6">
+        <v>42324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="F11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="6">
+        <v>42324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="F12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="6">
+        <v>42324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" ht="27" spans="1:7">
+        <v>31</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="6">
+        <v>42324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" ht="40.5" spans="1:7">
+        <v>31</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="6">
+        <v>42324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" ht="40.5" spans="1:7">
+        <v>31</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="6">
+        <v>42324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7">
+        <v>31</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="6">
+        <v>42324</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -934,7 +1262,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -946,57 +1274,55 @@
       <c r="G19" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="2:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B2" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="2:2">
-      <c r="B2" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Add question and fixed the pending question according to the answer in question list
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20370" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19440" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="问题" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="问题17" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <extLst/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
   <si>
     <t>编号</t>
   </si>
@@ -99,9 +98,6 @@
     <t>角色管理</t>
   </si>
   <si>
-    <t>角色对应权限列表里的移除权限的方法没有提供。</t>
-  </si>
-  <si>
     <t>2015.11.12</t>
   </si>
   <si>
@@ -201,13 +197,7 @@
     <t>没看到状况，新建的正常，是否为历史数据问题。</t>
   </si>
   <si>
-    <t>用户管理的搜索条件中有一个教工号，这个教工号是哪个字段？</t>
-  </si>
-  <si>
     <t>2015.11.16</t>
-  </si>
-  <si>
-    <t>对应的数据库里的“教工号”字段，接口中是“number”参数</t>
   </si>
   <si>
     <t>在专题提供的创建专题的接口里，只有三个入力参数
@@ -247,18 +237,42 @@
   <si>
     <t>按编码查询，结果集中编码项有重复</t>
   </si>
+  <si>
+    <t>资源管理和应用管理</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>在添加资源页面和添加专题页面的上传文件的功能中，上传问价的时候js报出下面的错误信息。
+XMLHttpRequest cannot load http://42.62.52.40:8000/file/upload. No 'Access-Control-Allow-Origin' header is present on the requested resource. Origin 'http://localhost:8080' is therefore not allowed access. 
+这个跨域访问的设置我在我这边设置后不起任何作用。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>耿晓红</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.11.19</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理的搜索条件中有一个教工号，这个教工号是哪个字段？</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>对应的数据库里的“教工号”字段，接口中是“number”参数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色对应权限列表里的移除权限的方法没有提供。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -287,8 +301,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -324,23 +339,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -372,23 +372,231 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4096" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="666750" y="352425"/>
+          <a:ext cx="9734550" cy="4695825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4097" name="图片 2" descr="rId2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="695325" y="5105400"/>
+          <a:ext cx="9858375" cy="5048250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3073" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6705600" cy="6400800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -686,6 +894,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -718,15 +927,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:G19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
     <col min="2" max="2" width="27.625" style="2" customWidth="1"/>
@@ -737,7 +945,7 @@
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -760,7 +968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="54" spans="1:7">
+    <row r="2" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -783,7 +991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" ht="54" spans="1:7">
+    <row r="3" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -806,7 +1014,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" ht="189" spans="1:7">
+    <row r="4" spans="1:7" ht="189" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -829,7 +1037,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" ht="27" spans="1:7">
+    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -852,383 +1060,653 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" ht="40.5" spans="1:7">
+    <row r="6" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>20</v>
+      <c r="C6" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G6" s="7">
         <v>42324</v>
       </c>
     </row>
-    <row r="7" ht="40.5" spans="1:7">
+    <row r="7" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" s="7">
         <v>42324</v>
       </c>
     </row>
-    <row r="8" ht="27" spans="1:7">
+    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="G8" s="7">
         <v>42324</v>
       </c>
     </row>
-    <row r="9" ht="54" spans="1:7">
+    <row r="9" spans="1:7" ht="54" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="G9" s="7">
         <v>42324</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="G10" s="7">
         <v>42324</v>
       </c>
     </row>
-    <row r="11" ht="27" spans="1:7">
+    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="7">
         <v>42324</v>
       </c>
     </row>
-    <row r="12" ht="27" spans="1:7">
+    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="G12" s="8">
         <v>42326</v>
       </c>
     </row>
-    <row r="13" ht="27" spans="1:7">
+    <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" s="8">
         <v>42326</v>
       </c>
     </row>
-    <row r="14" ht="27" spans="1:7">
+    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G14" s="7">
         <v>42324</v>
       </c>
     </row>
-    <row r="15" ht="40.5" spans="1:7">
+    <row r="15" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G15" s="7">
         <v>42324</v>
       </c>
     </row>
-    <row r="16" ht="40.5" spans="1:7">
+    <row r="16" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="E16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="G16" s="7">
         <v>42324</v>
       </c>
     </row>
-    <row r="17" ht="40.5" spans="1:7">
+    <row r="17" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>54</v>
+      <c r="C17" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="G17" s="7">
         <v>42326</v>
       </c>
     </row>
-    <row r="18" ht="256.5" spans="1:7">
+    <row r="18" spans="1:7" ht="256.5" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G18" s="7">
         <v>42326</v>
       </c>
     </row>
-    <row r="19" ht="27" spans="1:7">
+    <row r="19" spans="1:7" ht="27" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G19" s="7">
         <v>42326</v>
       </c>
     </row>
+    <row r="20" spans="1:7" ht="189" x14ac:dyDescent="0.15">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B2"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add question and commit code for resource
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19440" windowHeight="7920"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="问题" sheetId="1" r:id="rId1"/>
     <sheet name="问题15" sheetId="2" r:id="rId2"/>
     <sheet name="问题17" sheetId="3" r:id="rId3"/>
+    <sheet name="问题21" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="78">
   <si>
     <t>编号</t>
   </si>
@@ -155,49 +156,118 @@
     <t>资源管理</t>
   </si>
   <si>
+    <t>2015.11.15</t>
+  </si>
+  <si>
+    <t>创建资源接口的status参数是表示资源状态的</t>
+  </si>
+  <si>
+    <t>操作日志列表的接口没有提供</t>
+  </si>
+  <si>
+    <t>应用管理</t>
+  </si>
+  <si>
+    <t>应用管理相关的所有接口参数没有提供文档</t>
+  </si>
+  <si>
+    <t>应用管理目前只有专题的接口，先做专题</t>
+  </si>
+  <si>
+    <t>应该管理的页面下只有专题管理和精品课程管理，我们是只需要这两个功能吗？</t>
+  </si>
+  <si>
+    <t>同上</t>
+  </si>
+  <si>
+    <t>编码表</t>
+  </si>
+  <si>
+    <t>列表查询，按编码查询，结果集中编码项有重复，参见【问题15】sheet</t>
+  </si>
+  <si>
+    <t>田秋莲</t>
+  </si>
+  <si>
+    <t>没看到状况，新建的正常，是否为历史数据问题。</t>
+  </si>
+  <si>
+    <t>2015.11.16</t>
+  </si>
+  <si>
+    <t>2015.11.17</t>
+  </si>
+  <si>
+    <t>请查看最新的专题创建接口</t>
+  </si>
+  <si>
+    <t>词汇表</t>
+  </si>
+  <si>
+    <t>词汇表，更新前和更新后【词汇表】字段的顺序不一致</t>
+  </si>
+  <si>
+    <t>该问题已提交接口方</t>
+  </si>
+  <si>
+    <t>/encode?code=G</t>
+  </si>
+  <si>
+    <t>按编码查询，结果集中编码项有重复</t>
+  </si>
+  <si>
+    <t>资源管理和应用管理</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>在添加资源页面和添加专题页面的上传文件的功能中，上传问价的时候js报出下面的错误信息。
+XMLHttpRequest cannot load http://42.62.52.40:8000/file/upload. No 'Access-Control-Allow-Origin' header is present on the requested resource. Origin 'http://localhost:8080' is therefore not allowed access. 
+这个跨域访问的设置我在我这边设置后不起任何作用。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>耿晓红</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.11.19</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理的搜索条件中有一个教工号，这个教工号是哪个字段？</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>对应的数据库里的“教工号”字段，接口中是“number”参数</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色对应权限列表里的移除权限的方法没有提供。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>没有提供资源发布和审批的接口</t>
-  </si>
-  <si>
-    <t>2015.11.15</t>
-  </si>
-  <si>
-    <t>创建资源接口的status参数是表示资源状态的</t>
-  </si>
-  <si>
-    <t>操作日志列表的接口没有提供</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源管理</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>耿晓红</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.11.21</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>请参照 “日志统计访问”接口文档</t>
-  </si>
-  <si>
-    <t>应用管理</t>
-  </si>
-  <si>
-    <t>应用管理相关的所有接口参数没有提供文档</t>
-  </si>
-  <si>
-    <t>应用管理目前只有专题的接口，先做专题</t>
-  </si>
-  <si>
-    <t>应该管理的页面下只有专题管理和精品课程管理，我们是只需要这两个功能吗？</t>
-  </si>
-  <si>
-    <t>同上</t>
-  </si>
-  <si>
-    <t>编码表</t>
-  </si>
-  <si>
-    <t>列表查询，按编码查询，结果集中编码项有重复，参见【问题15】sheet</t>
-  </si>
-  <si>
-    <t>田秋莲</t>
-  </si>
-  <si>
-    <t>没看到状况，新建的正常，是否为历史数据问题。</t>
-  </si>
-  <si>
-    <t>2015.11.16</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源管理</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>在专题提供的创建专题的接口里，只有三个入力参数
@@ -215,56 +285,27 @@
   * 可否为空: yes
   * 说明：资源 id 列表
 但是在添加的popup上，有多余这三个参数的其他field，具体的参见sheet问题17.请确认添加的popup页面是否需要改变？</t>
-  </si>
-  <si>
-    <t>2015.11.17</t>
-  </si>
-  <si>
-    <t>请查看最新的专题创建接口</t>
-  </si>
-  <si>
-    <t>词汇表</t>
-  </si>
-  <si>
-    <t>词汇表，更新前和更新后【词汇表】字段的顺序不一致</t>
-  </si>
-  <si>
-    <t>该问题已提交接口方</t>
-  </si>
-  <si>
-    <t>/encode?code=G</t>
-  </si>
-  <si>
-    <t>按编码查询，结果集中编码项有重复</t>
-  </si>
-  <si>
-    <t>资源管理和应用管理</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>在添加资源页面和添加专题页面的上传文件的功能中，上传问价的时候js报出下面的错误信息。
-XMLHttpRequest cannot load http://42.62.52.40:8000/file/upload. No 'Access-Control-Allow-Origin' header is present on the requested resource. Origin 'http://localhost:8080' is therefore not allowed access. 
-这个跨域访问的设置我在我这边设置后不起任何作用。</t>
+    <t xml:space="preserve">更新资源的时候，按照最新的文档的参数传参，返回的是405， 请确认一下最新文档的参数是否正确。
+</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>耿晓红</t>
+    <t>操作日志的列表显示的mockup是要这样的吗？我现在用的是来源统计这个接口，如果这个不对，你能提供一下我们需要使用哪个具体的接口吗？还有，必须要和给定的表头一致吗？参见sheet【问题18】</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>2015.11.19</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户管理的搜索条件中有一个教工号，这个教工号是哪个字段？</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>对应的数据库里的“教工号”字段，接口中是“number”参数</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色对应权限列表里的移除权限的方法没有提供。</t>
+    <t>提供的表头</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>改完后的</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有找到相关资源源数据的接口，请确认这个接口。</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -272,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -304,6 +345,11 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -590,6 +636,121 @@
               <a:headEnd/>
               <a:tailEnd/>
             </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9525" y="180975"/>
+          <a:ext cx="7610475" cy="3905250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="4391025"/>
+          <a:ext cx="7105650" cy="1114425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -930,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1068,7 +1229,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>9</v>
@@ -1206,16 +1367,16 @@
         <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="G12" s="8">
         <v>42326</v>
@@ -1229,16 +1390,16 @@
         <v>38</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="G13" s="8">
         <v>42326</v>
@@ -1249,19 +1410,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G14" s="7">
         <v>42324</v>
@@ -1272,19 +1433,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G15" s="7">
         <v>42324</v>
@@ -1295,19 +1456,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="E16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="G16" s="7">
         <v>42324</v>
@@ -1321,16 +1482,16 @@
         <v>7</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G17" s="7">
         <v>42326</v>
@@ -1341,19 +1502,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G18" s="7">
         <v>42326</v>
@@ -1364,19 +1525,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="F19" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G19" s="7">
         <v>42326</v>
@@ -1387,44 +1548,74 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+    <row r="21" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+    <row r="22" spans="1:7" ht="81" x14ac:dyDescent="0.15">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+    <row r="23" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
@@ -1676,12 +1867,12 @@
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1697,7 +1888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1709,4 +1900,29 @@
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add question status and remark column
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="7890"/>
+    <workbookView windowWidth="20370" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="问题" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,12 @@
     <sheet name="问题21" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <extLst/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82">
   <si>
     <t>编号</t>
   </si>
@@ -38,6 +39,12 @@
   </si>
   <si>
     <t>回答时间</t>
+  </si>
+  <si>
+    <t>状态</t>
+  </si>
+  <si>
+    <t>备注</t>
   </si>
   <si>
     <t>用户管理</t>
@@ -77,10 +84,16 @@
     </r>
   </si>
   <si>
+    <t>已解决</t>
+  </si>
+  <si>
     <t>添加用户的时候，编号不能为空，如果为空，返回的content是序列号已经存在，这个逻辑应该是在后台实现的。</t>
   </si>
   <si>
     <t>编号不能为空，添加用户时需要填写</t>
+  </si>
+  <si>
+    <t>未解决</t>
   </si>
   <si>
     <t>部门管理</t>
@@ -93,12 +106,21 @@
     <t>测试未发现问题</t>
   </si>
   <si>
+    <t>需后台支持</t>
+  </si>
+  <si>
     <t>部门删除的模块也存在和3一样的问题。</t>
   </si>
   <si>
+    <t>后台已更新</t>
+  </si>
+  <si>
     <t>角色管理</t>
   </si>
   <si>
+    <t>角色对应权限列表里的移除权限的方法没有提供。</t>
+  </si>
+  <si>
     <t>2015.11.12</t>
   </si>
   <si>
@@ -156,6 +178,9 @@
     <t>资源管理</t>
   </si>
   <si>
+    <t>没有提供资源发布和审批的接口</t>
+  </si>
+  <si>
     <t>2015.11.15</t>
   </si>
   <si>
@@ -165,6 +190,12 @@
     <t>操作日志列表的接口没有提供</t>
   </si>
   <si>
+    <t>请参照 “日志统计访问”接口文档</t>
+  </si>
+  <si>
+    <t>参照问题21</t>
+  </si>
+  <si>
     <t>应用管理</t>
   </si>
   <si>
@@ -174,6 +205,9 @@
     <t>应用管理目前只有专题的接口，先做专题</t>
   </si>
   <si>
+    <t>只做专题</t>
+  </si>
+  <si>
     <t>应该管理的页面下只有专题管理和精品课程管理，我们是只需要这两个功能吗？</t>
   </si>
   <si>
@@ -192,82 +226,13 @@
     <t>没看到状况，新建的正常，是否为历史数据问题。</t>
   </si>
   <si>
+    <t>用户管理的搜索条件中有一个教工号，这个教工号是哪个字段？</t>
+  </si>
+  <si>
     <t>2015.11.16</t>
   </si>
   <si>
-    <t>2015.11.17</t>
-  </si>
-  <si>
-    <t>请查看最新的专题创建接口</t>
-  </si>
-  <si>
-    <t>词汇表</t>
-  </si>
-  <si>
-    <t>词汇表，更新前和更新后【词汇表】字段的顺序不一致</t>
-  </si>
-  <si>
-    <t>该问题已提交接口方</t>
-  </si>
-  <si>
-    <t>/encode?code=G</t>
-  </si>
-  <si>
-    <t>按编码查询，结果集中编码项有重复</t>
-  </si>
-  <si>
-    <t>资源管理和应用管理</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>在添加资源页面和添加专题页面的上传文件的功能中，上传问价的时候js报出下面的错误信息。
-XMLHttpRequest cannot load http://42.62.52.40:8000/file/upload. No 'Access-Control-Allow-Origin' header is present on the requested resource. Origin 'http://localhost:8080' is therefore not allowed access. 
-这个跨域访问的设置我在我这边设置后不起任何作用。</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>耿晓红</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>2015.11.19</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户管理的搜索条件中有一个教工号，这个教工号是哪个字段？</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>对应的数据库里的“教工号”字段，接口中是“number”参数</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色对应权限列表里的移除权限的方法没有提供。</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>没有提供资源发布和审批的接口</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>资源管理</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>耿晓红</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>2015.11.21</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>请参照 “日志统计访问”接口文档</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>资源管理</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>在专题提供的创建专题的接口里，只有三个入力参数
@@ -285,35 +250,70 @@
   * 可否为空: yes
   * 说明：资源 id 列表
 但是在添加的popup上，有多余这三个参数的其他field，具体的参见sheet问题17.请确认添加的popup页面是否需要改变？</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.11.17</t>
+  </si>
+  <si>
+    <t>请查看最新的专题创建接口</t>
+  </si>
+  <si>
+    <t>词汇表</t>
+  </si>
+  <si>
+    <t>词汇表，更新前和更新后【词汇表】字段的顺序不一致</t>
+  </si>
+  <si>
+    <t>该问题已提交接口方</t>
+  </si>
+  <si>
+    <t>资源管理和应用管理</t>
+  </si>
+  <si>
+    <t>在添加资源页面和添加专题页面的上传文件的功能中，上传问价的时候js报出下面的错误信息。
+XMLHttpRequest cannot load http://42.62.52.40:8000/file/upload. No 'Access-Control-Allow-Origin' header is present on the requested resource. Origin 'http://localhost:8080' is therefore not allowed access. 
+这个跨域访问的设置我在我这边设置后不起任何作用。</t>
+  </si>
+  <si>
+    <t>2015.11.19</t>
   </si>
   <si>
     <t xml:space="preserve">更新资源的时候，按照最新的文档的参数传参，返回的是405， 请确认一下最新文档的参数是否正确。
 </t>
-    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.11.21</t>
+  </si>
+  <si>
+    <t>操作日志的列表显示的mockup是要这样的吗？我现在用的是来源统计这个接口，如果这个不对，你能提供一下我们需要使用哪个具体的接口吗？还有，必须要和给定的表头一致吗？参见sheet【问题21】</t>
+  </si>
+  <si>
+    <t>没有找到相关资源元数据编辑的接口，请确认这个接口。</t>
+  </si>
+  <si>
+    <t>/encode?code=G</t>
+  </si>
+  <si>
+    <t>按编码查询，结果集中编码项有重复</t>
+  </si>
+  <si>
+    <t>改完后的</t>
   </si>
   <si>
     <t>提供的表头</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>改完后的</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>没有找到相关资源元数据编辑的接口，请确认这个接口。</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>操作日志的列表显示的mockup是要这样的吗？我现在用的是来源统计这个接口，如果这个不对，你能提供一下我们需要使用哪个具体的接口吗？还有，必须要和给定的表头一致吗？参见sheet【问题21】</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -342,13 +342,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -361,7 +355,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -384,13 +378,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -399,365 +421,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="百分比" xfId="4" builtinId="5"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4096" name="图片 1" descr="rId1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="666750" y="352425"/>
-          <a:ext cx="9734550" cy="4695825"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4097" name="图片 2" descr="rId2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="695325" y="5105400"/>
-          <a:ext cx="9858375" cy="5048250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3073" name="图片 1" descr="rId1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="6705600" cy="6400800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9525" y="180975"/>
-          <a:ext cx="7610475" cy="3905250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="4391025"/>
-          <a:ext cx="7105650" cy="1114425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1055,7 +767,6 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -1088,16 +799,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="2"/>
+    <col min="1" max="1" width="4.55833333333333" style="2" customWidth="1"/>
     <col min="2" max="2" width="27.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.875" style="2" customWidth="1"/>
     <col min="4" max="5" width="22.25" style="2" customWidth="1"/>
@@ -1106,7 +820,7 @@
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1125,804 +839,975 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="54" x14ac:dyDescent="0.15">
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" ht="54" spans="1:13">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="54" x14ac:dyDescent="0.15">
+        <v>13</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="M2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" ht="54" spans="1:13">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="189" x14ac:dyDescent="0.15">
+      <c r="H3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="M3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" ht="189" spans="1:13">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="I4" s="5"/>
+      <c r="M4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" ht="27" spans="1:13">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="I5" s="5"/>
+      <c r="M5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" ht="40.5" spans="1:9">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>65</v>
+        <v>25</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="7">
+        <v>28</v>
+      </c>
+      <c r="G6" s="10">
         <v>42324</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="H6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" ht="40.5" spans="1:9">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="7">
+        <v>31</v>
+      </c>
+      <c r="G7" s="10">
         <v>42324</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="H7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" ht="27" spans="1:9">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="7">
+        <v>36</v>
+      </c>
+      <c r="G8" s="10">
         <v>42324</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="54" x14ac:dyDescent="0.15">
+      <c r="H8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" ht="54" spans="1:9">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="7">
+        <v>39</v>
+      </c>
+      <c r="G9" s="10">
         <v>42324</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="7">
+        <v>42</v>
+      </c>
+      <c r="G10" s="10">
         <v>42324</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" ht="27" spans="1:9">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="7">
+        <v>39</v>
+      </c>
+      <c r="G11" s="10">
         <v>42324</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="H11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" ht="27" spans="1:9">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="8">
+        <v>48</v>
+      </c>
+      <c r="G12" s="11">
         <v>42326</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="H12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" ht="27" spans="1:9">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="8">
+        <v>50</v>
+      </c>
+      <c r="G13" s="11">
         <v>42326</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="H13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" ht="27" spans="1:9">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="7">
+        <v>54</v>
+      </c>
+      <c r="G14" s="10">
         <v>42324</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="H14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" ht="40.5" spans="1:9">
       <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="7">
+        <v>57</v>
+      </c>
+      <c r="G15" s="10">
         <v>42324</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="H15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" ht="40.5" spans="1:9">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="7">
+        <v>61</v>
+      </c>
+      <c r="G16" s="10">
         <v>42324</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="H16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" ht="40.5" spans="1:9">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="10">
         <v>42326</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="256.5" x14ac:dyDescent="0.15">
+      <c r="H17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" ht="256.5" spans="1:9">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="7">
+        <v>67</v>
+      </c>
+      <c r="G18" s="10">
         <v>42326</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="H18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" ht="27" spans="1:9">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>49</v>
+        <v>69</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="7">
+        <v>70</v>
+      </c>
+      <c r="G19" s="10">
         <v>42326</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="189" x14ac:dyDescent="0.15">
+      <c r="H19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" ht="189" spans="1:9">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="G20" s="4"/>
+      <c r="H20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" ht="67.5" spans="1:9">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="81" x14ac:dyDescent="0.15">
+      <c r="G21" s="4"/>
+      <c r="H21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" ht="81" spans="1:9">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="G22" s="4"/>
+      <c r="H22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" ht="27" spans="1:9">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G23" s="4"/>
+      <c r="H23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G24" s="4"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G25" s="4"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G27" s="4"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G28" s="4"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G29" s="4"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G30" s="4"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G31" s="4"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G32" s="4"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G33" s="4"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G34" s="4"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G35" s="4"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G36" s="4"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G37" s="4"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G38" s="4"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G39" s="4"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G40" s="4"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G41" s="4"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G42" s="4"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G43" s="4"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G44" s="4"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G45" s="4"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G46" s="4"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G47" s="4"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2 H3 H4 H5 H6 H7 H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38 H39 H40 H41 H42 H43 H44 H45 H46 H47 H48">
+      <formula1>$M$2:$M$5</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="B1:B2"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:2">
       <c r="B1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update questionList answer 20151123
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106">
   <si>
     <t>编号</t>
   </si>
@@ -91,7 +91,35 @@
     <t>添加用户的时候，编号不能为空，如果为空，返回的content是序列号已经存在，这个逻辑应该是在后台实现的。</t>
   </si>
   <si>
-    <t>编号不能为空，添加用户时需要填写</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>编号不能为空,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>不可重复</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，添加用户时需要填写</t>
+    </r>
   </si>
   <si>
     <t>未解决</t>
@@ -159,6 +187,9 @@
   </si>
   <si>
     <t>接口问题，马上提交进行调整</t>
+  </si>
+  <si>
+    <t>已测试，True、False首字母大写</t>
   </si>
   <si>
     <t>标签管理</t>
@@ -279,6 +310,9 @@
     <t>2015.11.19</t>
   </si>
   <si>
+    <t>接口貌似有所调整，待反馈</t>
+  </si>
+  <si>
     <t xml:space="preserve">更新资源的时候，按照最新的文档的参数传参，返回的是405， 请确认一下最新文档的参数是否正确。
 </t>
   </si>
@@ -286,30 +320,51 @@
     <t>2015.11.21</t>
   </si>
   <si>
+    <t>测试正常</t>
+  </si>
+  <si>
     <t>操作日志的列表显示的mockup是要这样的吗？我现在用的是来源统计这个接口，如果这个不对，你能提供一下我们需要使用哪个具体的接口吗？还有，必须要和给定的表头一致吗？参见sheet【问题21】</t>
   </si>
   <si>
+    <t>您调用的是统计接口，针对资源操作日志，需要一个额外的接口，目前未实现。</t>
+  </si>
+  <si>
     <t>没有找到相关资源元数据编辑的接口，请确认这个接口。</t>
   </si>
   <si>
+    <t>参见《资源库和资源相关文档》最后部分</t>
+  </si>
+  <si>
     <t>关于角色对应权限列表里的权限移除，我还有疑问。请参照sheet【问题23】</t>
   </si>
   <si>
+    <t>当前ui端实现的与接口设计不相符。设计的流程是这样：权限不提供修改接口，只有新建和删除。删除权限不需要删除角色，角色是可以修改的。</t>
+  </si>
+  <si>
     <t>结构类型</t>
   </si>
   <si>
     <t>列表中有checkbox，是否需要批量删除功能？目前接口文档中没有批量删除接口，如果需要批量删除，请提供批量删除接口。</t>
   </si>
   <si>
+    <t>不用批量删除，逐条删除需用户确认</t>
+  </si>
+  <si>
     <t>元数据</t>
   </si>
   <si>
     <t>元数据分类和标准tree返回的node_type 都是1，导致不能区分是元数据分类还是元数据标准，致使无法增加元数据</t>
   </si>
   <si>
+    <t>确实存在这个问题，已经提交接口方处理</t>
+  </si>
+  <si>
     <t>元数据列表查询处，第一个下拉款【必选元素】【可选元素】【分类元素】代表什么? 第一个下拉框是和第二个下框有没有级联关系？</t>
   </si>
   <si>
+    <t>必选元素、可选元素、分类元素是CELTS标准中对元数据标准的分类描述，相当于标准中的元数据项进行分类，没有层级关系</t>
+  </si>
+  <si>
     <t>Web服务配置</t>
   </si>
   <si>
@@ -317,6 +372,9 @@
   </si>
   <si>
     <t>2015.11.22</t>
+  </si>
+  <si>
+    <t>接口正在实现中</t>
   </si>
   <si>
     <t>流媒体服务</t>
@@ -354,10 +412,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -846,9 +904,9 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -859,7 +917,9 @@
     <col min="4" max="5" width="22.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="8" max="8" width="9" style="1"/>
+    <col min="9" max="9" width="20" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -937,7 +997,7 @@
       <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -1117,17 +1177,19 @@
       <c r="H9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>34</v>
@@ -1136,7 +1198,7 @@
         <v>35</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G10" s="9">
         <v>42324</v>
@@ -1149,10 +1211,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>34</v>
@@ -1169,26 +1231,28 @@
       <c r="H11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" ht="27" spans="1:9">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G12" s="10">
         <v>42326</v>
@@ -1203,19 +1267,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="G13" s="10">
         <v>42326</v>
@@ -1224,7 +1288,7 @@
         <v>18</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" ht="27" spans="1:9">
@@ -1232,19 +1296,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G14" s="9">
         <v>42324</v>
@@ -1253,7 +1317,7 @@
         <v>15</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" ht="40.5" spans="1:9">
@@ -1261,19 +1325,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G15" s="9">
         <v>42324</v>
@@ -1282,7 +1346,7 @@
         <v>15</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" ht="40.5" spans="1:9">
@@ -1290,19 +1354,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G16" s="9">
         <v>42324</v>
@@ -1320,16 +1384,16 @@
         <v>9</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G17" s="9">
         <v>42326</v>
@@ -1344,19 +1408,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G18" s="9">
         <v>42326</v>
@@ -1371,19 +1435,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G19" s="9">
         <v>42326</v>
@@ -1398,19 +1462,23 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="3" t="s">
         <v>72</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="9">
+        <v>42331</v>
+      </c>
       <c r="H20" s="3" t="s">
         <v>18</v>
       </c>
@@ -1421,42 +1489,50 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>74</v>
+        <v>46</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="9">
+        <v>42331</v>
+      </c>
       <c r="H21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="22" ht="81" spans="1:9">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>76</v>
+        <v>46</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="9">
+        <v>42331</v>
+      </c>
       <c r="H22" s="3" t="s">
         <v>18</v>
       </c>
@@ -1467,25 +1543,29 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>77</v>
+        <v>46</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="9">
+        <v>42331</v>
+      </c>
       <c r="H23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" ht="40.5" spans="1:9">
+      <c r="I23" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" ht="81" spans="1:9">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1493,16 +1573,20 @@
         <v>25</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="9">
+        <v>42331</v>
+      </c>
       <c r="H24" s="3" t="s">
         <v>18</v>
       </c>
@@ -1513,19 +1597,23 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="9">
+        <v>42331</v>
+      </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
@@ -1534,61 +1622,73 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G26" s="9">
+        <v>42331</v>
+      </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" ht="54" spans="1:9">
+    <row r="27" ht="81" spans="1:9">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F27" s="3"/>
-      <c r="G27" s="4"/>
+      <c r="G27" s="9">
+        <v>42331</v>
+      </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="9">
+        <v>42331</v>
+      </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
@@ -1597,19 +1697,23 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="9">
+        <v>42331</v>
+      </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
@@ -1618,19 +1722,23 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="4"/>
+        <v>95</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" s="9">
+        <v>42331</v>
+      </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
@@ -1834,7 +1942,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H48">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H30 H31:H48">
       <formula1>$M$2:$M$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -1860,12 +1968,12 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="2:2">
       <c r="B2" s="2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1909,12 +2017,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1943,7 +2051,7 @@
     <row r="13" ht="35.25" customHeight="1"/>
     <row r="14" ht="81" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add question for topic management.
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20370" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="问题" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,11 @@
     <sheet name="问题【23】" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <extLst/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="110">
   <si>
     <t>编号</t>
   </si>
@@ -406,18 +405,33 @@
 我试着使用http://42.62.52.40:8000/role/role.node/permission/id， 例如：http://42.62.52.40:8000/role/21/permission/1，但是结果返回的是404. 请帮忙确认
 这个问题，谢谢。</t>
   </si>
+  <si>
+    <t>应用管理</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加专题的接口参数在文档定义如下：
+is_publish
+  * type: boolean
+  * 举例: "0","1"
+  * 可否为空: yes, 默认值为0，表示该专题不可发布
+我这边传的参数选择发布的时候参数值为1,选择禁用时参数值为0，但是无论我传哪个参数，接口返回的结果都是true。请帮忙确认这个接口返回值的正确性。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>耿晓红</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.11.24</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -443,6 +457,11 @@
       <color indexed="10"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -491,23 +510,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -545,31 +549,445 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8190" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="666750" y="352425"/>
+          <a:ext cx="9734550" cy="4695825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8191" name="图片 2" descr="rId2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="695325" y="5105400"/>
+          <a:ext cx="9858375" cy="5048250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10240" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6705600" cy="6400800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11266" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9525" y="180975"/>
+          <a:ext cx="7610475" cy="3905250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11265" name="图片 2" descr="rId2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="4391025"/>
+          <a:ext cx="7105650" cy="1114425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9934575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5121" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9934575" cy="2171700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -867,6 +1285,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -899,17 +1318,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.625" style="1" customWidth="1"/>
@@ -922,7 +1339,7 @@
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -951,7 +1368,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="54" spans="1:13">
+    <row r="2" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -981,7 +1398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" ht="54" spans="1:13">
+    <row r="3" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1011,7 +1428,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" ht="189" spans="1:13">
+    <row r="4" spans="1:13" ht="189" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1041,7 +1458,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" ht="27" spans="1:13">
+    <row r="5" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1071,7 +1488,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" ht="40.5" spans="1:9">
+    <row r="6" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1098,7 +1515,7 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" ht="40.5" spans="1:9">
+    <row r="7" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1125,7 +1542,7 @@
       </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" ht="27" spans="1:9">
+    <row r="8" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1152,7 +1569,7 @@
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" ht="54" spans="1:9">
+    <row r="9" spans="1:13" ht="54" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1181,7 +1598,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1206,7 +1623,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" ht="27" spans="1:9">
+    <row r="11" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1235,7 +1652,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" ht="27" spans="1:9">
+    <row r="12" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1262,7 +1679,7 @@
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" ht="27" spans="1:9">
+    <row r="13" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1291,7 +1708,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" ht="27" spans="1:9">
+    <row r="14" spans="1:13" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1320,7 +1737,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" ht="40.5" spans="1:9">
+    <row r="15" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1349,7 +1766,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" ht="40.5" spans="1:9">
+    <row r="16" spans="1:13" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1376,7 +1793,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" ht="40.5" spans="1:9">
+    <row r="17" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1403,7 +1820,7 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" ht="256.5" spans="1:9">
+    <row r="18" spans="1:9" ht="256.5" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1430,7 +1847,7 @@
       </c>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" ht="27" spans="1:9">
+    <row r="19" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1457,7 +1874,7 @@
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" ht="189" spans="1:9">
+    <row r="20" spans="1:9" ht="189" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1484,7 +1901,7 @@
       </c>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" ht="67.5" spans="1:9">
+    <row r="21" spans="1:9" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1511,7 +1928,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" ht="81" spans="1:9">
+    <row r="22" spans="1:9" ht="81" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1538,7 +1955,7 @@
       </c>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" ht="27" spans="1:9">
+    <row r="23" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1565,7 +1982,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" ht="81" spans="1:9">
+    <row r="24" spans="1:9" ht="81" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1592,7 +2009,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" ht="54" spans="1:9">
+    <row r="25" spans="1:9" ht="54" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1617,7 +2034,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" ht="54" spans="1:9">
+    <row r="26" spans="1:9" ht="54" x14ac:dyDescent="0.15">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1642,7 +2059,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" ht="81" spans="1:9">
+    <row r="27" spans="1:9" ht="81" x14ac:dyDescent="0.15">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -1667,7 +2084,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1692,7 +2109,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1717,7 +2134,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1742,18 +2159,28 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+    <row r="31" spans="1:9" ht="162" x14ac:dyDescent="0.15">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="4"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1764,7 +2191,7 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1775,7 +2202,7 @@
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1786,7 +2213,7 @@
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1797,7 +2224,7 @@
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1808,7 +2235,7 @@
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1819,7 +2246,7 @@
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1830,7 +2257,7 @@
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1841,7 +2268,7 @@
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1852,7 +2279,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1863,7 +2290,7 @@
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1874,7 +2301,7 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1885,7 +2312,7 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1896,7 +2323,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1907,7 +2334,7 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1918,7 +2345,7 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1929,7 +2356,7 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1941,124 +2368,119 @@
       <c r="I48" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H30 H31:H48">
       <formula1>$M$2:$M$5</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B2"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B1" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B2" s="2" t="s">
         <v>102</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A13:A14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="135.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" ht="35.25" customHeight="1"/>
-    <row r="14" ht="81" spans="1:1">
+    <row r="13" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:1" ht="81" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change code for topic function
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20370" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="问题" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">问题!$A$1:$M$44</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <extLst/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="151">
   <si>
     <t>编号</t>
   </si>
@@ -545,18 +544,24 @@
   <si>
     <t>页面列名</t>
   </si>
+  <si>
+    <t>资源管理</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.12.2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于问题33， 是资源管理当中的元数据编辑，我这边调用接口后，返回200，但是数据没有任何更新。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -585,16 +590,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="20"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="12"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -644,29 +640,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -707,45 +682,1046 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12284" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="666750" y="352425"/>
+          <a:ext cx="9734550" cy="4695825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12285" name="图片 2" descr="rId2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="695325" y="5105400"/>
+          <a:ext cx="9858375" cy="5048250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16382" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6705600" cy="6400800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19456" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9525" y="180975"/>
+          <a:ext cx="7610475" cy="3905250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19455" name="图片 2" descr="rId2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="4391025"/>
+          <a:ext cx="7105650" cy="1114425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9934575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21504" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9934575" cy="2171700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6146" name="图片 2" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="647700" y="704850"/>
+          <a:ext cx="7315200" cy="4114800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6147" name="矩形 3"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1695450" y="1571625"/>
+          <a:ext cx="2390775" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="0"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:miter lim="200000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6149" name="图片 5" descr="rId2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="647700" y="5143500"/>
+          <a:ext cx="7315200" cy="4114800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6150" name="矩形 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1685925" y="5838825"/>
+          <a:ext cx="2390775" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000">
+            <a:alpha val="0"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7169" name="图片 1" descr="rId1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="695325" y="342900"/>
+          <a:ext cx="8239125" cy="4629150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7170" name="矩形 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="647700" y="3028950"/>
+          <a:ext cx="8543925" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:miter lim="200000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="BBD5F0">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8196" name="组合 4"/>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1400175" y="552450"/>
+          <a:ext cx="8143875" cy="4572000"/>
+          <a:chOff x="2182" y="795"/>
+          <a:chExt cx="12830" cy="7214"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="8193" name="图片 1" descr="rId1"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="2182" y="795"/>
+            <a:ext cx="12830" cy="7214"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+            <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:miter lim="800000"/>
+                <a:headEnd/>
+                <a:tailEnd/>
+              </a14:hiddenLine>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8194" name="矩形 2"/>
+          <xdr:cNvSpPr>
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="5205" y="4560"/>
+            <a:ext cx="8490" cy="2460"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="15875">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:miter lim="200000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="BBD5F0">
+                    <a:alpha val="0"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8200" name="组合 8"/>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1390650" y="5476875"/>
+          <a:ext cx="9448800" cy="5305425"/>
+          <a:chOff x="2198" y="8626"/>
+          <a:chExt cx="14884" cy="8368"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="8197" name="图片 5" descr="rId2"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="2198" y="8626"/>
+            <a:ext cx="14884" cy="8369"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+            <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:miter lim="800000"/>
+                <a:headEnd/>
+                <a:tailEnd/>
+              </a14:hiddenLine>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8198" name="矩形 6"/>
+          <xdr:cNvSpPr>
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="4395" y="10545"/>
+            <a:ext cx="12585" cy="870"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="15875">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:miter lim="200000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="BBD5F0"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1043,6 +2019,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -1075,17 +2052,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="4.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="27.625" style="2" customWidth="1"/>
@@ -1098,7 +2074,7 @@
     <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" spans="1:9">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +2103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" ht="54" hidden="1" spans="1:13">
+    <row r="2" spans="1:13" ht="54" hidden="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1153,14 +2129,11 @@
         <v>15</v>
       </c>
       <c r="I2" s="4"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
       <c r="M2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" ht="54" hidden="1" spans="1:13">
+    <row r="3" spans="1:13" ht="54" hidden="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1186,14 +2159,11 @@
         <v>15</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="1" ht="189" hidden="1" spans="1:13">
+    <row r="4" spans="1:13" ht="189" hidden="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1219,14 +2189,11 @@
         <v>15</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="1" ht="27" hidden="1" spans="1:13">
+    <row r="5" spans="1:13" ht="27" hidden="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1252,14 +2219,11 @@
         <v>15</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="1" ht="40.5" hidden="1" spans="1:9">
+    <row r="6" spans="1:13" ht="40.5" hidden="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1286,7 +2250,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" s="2" customFormat="1" ht="40.5" hidden="1" spans="1:9">
+    <row r="7" spans="1:13" ht="40.5" hidden="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1313,7 +2277,7 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" s="2" customFormat="1" ht="27" hidden="1" spans="1:9">
+    <row r="8" spans="1:13" ht="27" hidden="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1340,7 +2304,7 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" s="2" customFormat="1" ht="54" hidden="1" spans="1:9">
+    <row r="9" spans="1:13" ht="54" hidden="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1369,7 +2333,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="1" hidden="1" spans="1:9">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1396,7 +2360,7 @@
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" s="2" customFormat="1" ht="27" hidden="1" spans="1:9">
+    <row r="11" spans="1:13" ht="27" hidden="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1425,7 +2389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" s="2" customFormat="1" ht="27" hidden="1" spans="1:9">
+    <row r="12" spans="1:13" ht="27" hidden="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1452,7 +2416,7 @@
       </c>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" s="2" customFormat="1" ht="27" hidden="1" spans="1:9">
+    <row r="13" spans="1:13" ht="27" hidden="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1481,7 +2445,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" s="2" customFormat="1" ht="27" hidden="1" spans="1:9">
+    <row r="14" spans="1:13" ht="27" hidden="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1510,7 +2474,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" s="2" customFormat="1" ht="40.5" hidden="1" spans="1:9">
+    <row r="15" spans="1:13" ht="40.5" hidden="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1539,7 +2503,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" s="2" customFormat="1" ht="40.5" hidden="1" spans="1:9">
+    <row r="16" spans="1:13" ht="40.5" hidden="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1566,7 +2530,7 @@
       </c>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" s="2" customFormat="1" ht="40.5" hidden="1" spans="1:9">
+    <row r="17" spans="1:9" ht="40.5" hidden="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1593,7 +2557,7 @@
       </c>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" s="2" customFormat="1" ht="256.5" hidden="1" spans="1:9">
+    <row r="18" spans="1:9" ht="256.5" hidden="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1620,7 +2584,7 @@
       </c>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" s="2" customFormat="1" ht="27" hidden="1" spans="1:9">
+    <row r="19" spans="1:9" ht="27" hidden="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1649,7 +2613,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" s="2" customFormat="1" ht="189" spans="1:9">
+    <row r="20" spans="1:9" ht="189" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1678,7 +2642,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" s="2" customFormat="1" ht="67.5" hidden="1" spans="1:9">
+    <row r="21" spans="1:9" ht="67.5" hidden="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1705,7 +2669,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" s="2" customFormat="1" ht="81" spans="1:9">
+    <row r="22" spans="1:9" ht="81" x14ac:dyDescent="0.15">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1734,7 +2698,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" s="2" customFormat="1" ht="27" hidden="1" spans="1:9">
+    <row r="23" spans="1:9" ht="27" hidden="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1761,7 +2725,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" s="2" customFormat="1" ht="81" hidden="1" spans="1:9">
+    <row r="24" spans="1:9" ht="81" hidden="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1788,7 +2752,7 @@
       </c>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" s="2" customFormat="1" ht="54" hidden="1" spans="1:9">
+    <row r="25" spans="1:9" ht="54" hidden="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1815,7 +2779,7 @@
       </c>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" s="2" customFormat="1" ht="54" hidden="1" spans="1:9">
+    <row r="26" spans="1:9" ht="54" hidden="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1844,7 +2808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" s="2" customFormat="1" ht="67.5" hidden="1" spans="1:9">
+    <row r="27" spans="1:9" ht="67.5" hidden="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -1871,7 +2835,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" s="2" customFormat="1" ht="27" spans="1:9">
+    <row r="28" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1900,7 +2864,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" s="2" customFormat="1" ht="27" spans="1:9">
+    <row r="29" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -1929,7 +2893,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" s="2" customFormat="1" ht="27" spans="1:9">
+    <row r="30" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1958,7 +2922,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" s="2" customFormat="1" ht="162" hidden="1" spans="1:9">
+    <row r="31" spans="1:9" ht="162" hidden="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1983,7 +2947,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" s="2" customFormat="1" ht="40.5" hidden="1" spans="1:9">
+    <row r="32" spans="1:9" ht="40.5" hidden="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -2008,7 +2972,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" s="2" customFormat="1" ht="135" spans="1:9">
+    <row r="33" spans="1:9" ht="135" x14ac:dyDescent="0.15">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -2035,7 +2999,7 @@
       </c>
       <c r="I33" s="4"/>
     </row>
-    <row r="34" s="2" customFormat="1" ht="54" spans="1:9">
+    <row r="34" spans="1:9" ht="54" x14ac:dyDescent="0.15">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -2062,7 +3026,7 @@
       </c>
       <c r="I34" s="4"/>
     </row>
-    <row r="35" s="2" customFormat="1" ht="54" spans="1:9">
+    <row r="35" spans="1:9" ht="54" x14ac:dyDescent="0.15">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -2089,7 +3053,7 @@
       </c>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" s="2" customFormat="1" ht="27" spans="1:9">
+    <row r="36" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -2118,7 +3082,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" s="2" customFormat="1" ht="27" spans="1:9">
+    <row r="37" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -2147,7 +3111,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" s="2" customFormat="1" ht="94.5" spans="1:9">
+    <row r="38" spans="1:9" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -2174,7 +3138,7 @@
       </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" s="2" customFormat="1" ht="54" spans="1:9">
+    <row r="39" spans="1:9" ht="54" x14ac:dyDescent="0.15">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -2201,7 +3165,7 @@
       </c>
       <c r="I39" s="4"/>
     </row>
-    <row r="40" s="2" customFormat="1" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -2228,7 +3192,7 @@
       </c>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" s="2" customFormat="1" ht="67.5" spans="1:9">
+    <row r="41" spans="1:9" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -2255,7 +3219,7 @@
       </c>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" s="2" customFormat="1" ht="27" spans="1:9">
+    <row r="42" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -2282,7 +3246,7 @@
       </c>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" s="2" customFormat="1" ht="27" spans="1:9">
+    <row r="43" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -2309,7 +3273,7 @@
       </c>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" s="2" customFormat="1" ht="54" spans="1:9">
+    <row r="44" spans="1:9" ht="54" x14ac:dyDescent="0.15">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -2336,18 +3300,28 @@
       </c>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
+    <row r="45" spans="1:9" ht="54" x14ac:dyDescent="0.15">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="F45" s="4"/>
       <c r="G45" s="5"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2358,7 +3332,7 @@
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2369,7 +3343,7 @@
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2380,7 +3354,7 @@
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2391,7 +3365,7 @@
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2405,224 +3379,214 @@
   </sheetData>
   <autoFilter ref="A1:M44">
     <filterColumn colId="7">
-      <customFilters>
-        <customFilter operator="equal" val="未解决"/>
-      </customFilters>
+      <filters>
+        <filter val="未解决"/>
+      </filters>
     </filterColumn>
   </autoFilter>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H44 H45:H50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H50">
       <formula1>$M$2:$M$5</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A29:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2">
+    <row r="1" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B1" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B2" s="3" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>140</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A13:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="135.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" ht="35.25" customHeight="1"/>
-    <row r="14" ht="81" spans="1:1">
+    <row r="13" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:1" ht="81" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>141</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="2:2">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
         <v>143</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B3"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B2" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B3">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C32"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="3:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="32" spans="3:3">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.15">
       <c r="C32" t="s">
         <v>147</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change code for user and topic module.
</commit_message>
<xml_diff>
--- a/doc/Question List.xlsx
+++ b/doc/Question List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="152">
   <si>
     <t>编号</t>
   </si>
@@ -543,6 +543,22 @@
   </si>
   <si>
     <t>当前ui端实现的与接口设计不相符。设计的流程是这样：权限不提供修改接口，只有新建和删除。删除权限不需要删除角色，角色是可以修改的。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆页面</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>登陆页面只能使用superadmin登陆，我自己新建的用户，输入的用户名和密码都正确，但是返回的错误信息是：“用户名和密码不匹配”，请确认这个问题。</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>耿晓红</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015.12.11</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -2046,8 +2062,8 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3289,12 +3305,22 @@
       </c>
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
+    <row r="45" spans="1:9" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A45" s="4">
+        <v>35</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="F45" s="4"/>
       <c r="G45" s="5"/>
       <c r="H45" s="4"/>

</xml_diff>